<commit_message>
test cigna global health
</commit_message>
<xml_diff>
--- a/Input/Cigna_Global_Health/userType.xlsx
+++ b/Input/Cigna_Global_Health/userType.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t xml:space="preserve">benefits</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t xml:space="preserve">Emergency-Evacuation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repatriation-Benefit</t>
   </si>
   <si>
     <t xml:space="preserve">Virtual / Tele Doctor</t>
@@ -262,10 +265,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -546,15 +549,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -562,7 +565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>40</v>
       </c>
@@ -578,12 +581,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
         <v>43</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>